<commit_message>
fixed measurement output with names to match columns with unique ID
</commit_message>
<xml_diff>
--- a/Scallop_Invoice_template2.xlsx
+++ b/Scallop_Invoice_template2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1_LAB OPERATIONS_authorized access only\INVERTEBRATES\Scallop\Scallop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD958A14-4DF2-4470-860F-C134FDAD8A08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1BF9D9-BF2D-495D-BB32-C1908E9E5094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8280" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample invoice form" sheetId="1" r:id="rId1"/>
@@ -117,10 +117,10 @@
     <t>ADFG</t>
   </si>
   <si>
-    <t>Ryan Burt</t>
+    <t>STRUCTURE</t>
   </si>
   <si>
-    <t>STRUCTURE</t>
+    <t>Alyssa Hopkins</t>
   </si>
 </sst>
 </file>
@@ -162,6 +162,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -429,6 +430,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -472,24 +491,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,8 +1082,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q1352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,13 +1125,12 @@
       <c r="L1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="N1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="26"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
@@ -1149,13 +1149,12 @@
       <c r="L2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="29">
+      <c r="N2" s="14">
         <v>4</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="27"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="33"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41"/>
@@ -1172,80 +1171,79 @@
       <c r="L3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="29" t="s">
-        <v>27</v>
+      <c r="N3" s="14" t="s">
+        <v>28</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="27"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="33"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="32"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="28"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="22"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="17" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="20" t="s">
+      <c r="M6" s="24"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="22"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="28"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1288,7 +1286,7 @@
         <v>14</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>15</v>
@@ -26636,20 +26634,16 @@
       <c r="P1352"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="9">
     <mergeCell ref="A5:Q5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="O6:Q6"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M4:P4"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
-    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -26661,8 +26655,58 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId4" name="Control 4">
+        <control shapeId="1025" r:id="rId4" name="Control 1">
           <controlPr defaultSize="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>733425</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId4" name="Control 1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1026" r:id="rId6" name="Control 2">
+          <controlPr defaultSize="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>733425</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>180975</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1026" r:id="rId6" name="Control 2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1027" r:id="rId8" name="Control 3">
+          <controlPr defaultSize="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -26681,13 +26725,13 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1028" r:id="rId4" name="Control 4"/>
+        <control shapeId="1027" r:id="rId8" name="Control 3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1027" r:id="rId6" name="Control 3">
-          <controlPr defaultSize="0" r:id="rId7">
+        <control shapeId="1028" r:id="rId10" name="Control 4">
+          <controlPr defaultSize="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -26706,57 +26750,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1027" r:id="rId6" name="Control 3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId8" name="Control 2">
-          <controlPr defaultSize="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>733425</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1026" r:id="rId8" name="Control 2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId10" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>733425</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>180975</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId10" name="Control 1"/>
+        <control shapeId="1028" r:id="rId10" name="Control 4"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -26764,12 +26758,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26887,15 +26878,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA2D53D-40E7-4881-BAA3-C747EC9E07F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D3B3AA-6A35-4478-BB4A-3930B3EA9A78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -26917,16 +26918,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D3B3AA-6A35-4478-BB4A-3930B3EA9A78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FA2D53D-40E7-4881-BAA3-C747EC9E07F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>